<commit_message>
Loinc rules for June
</commit_message>
<xml_diff>
--- a/isaac-db-processing-rules/src/main/resources/SOLOR LOINC Rules.xlsx
+++ b/isaac-db-processing-rules/src/main/resources/SOLOR LOINC Rules.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="959" uniqueCount="362">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1217" uniqueCount="446">
   <si>
     <t>ID</t>
   </si>
@@ -1102,15 +1102,268 @@
   </si>
   <si>
     <t>measurement of Western equine encephalitis virus antibody (procedure)</t>
+  </si>
+  <si>
+    <t>Immune complex</t>
+  </si>
+  <si>
+    <t>immune complex assay (procedure)</t>
+  </si>
+  <si>
+    <t>Epstein Barr virus DNA</t>
+  </si>
+  <si>
+    <t>Epstein Barr virus deoxyribonucleic acid assay (procedure)</t>
+  </si>
+  <si>
+    <t>Manganese</t>
+  </si>
+  <si>
+    <t>manganese measurement (procedure)</t>
+  </si>
+  <si>
+    <t>Carnitine</t>
+  </si>
+  <si>
+    <t>carnitine measurement (procedure)</t>
+  </si>
+  <si>
+    <t>La Crosse virus Ab</t>
+  </si>
+  <si>
+    <t>measurement of La Crosse virus antibody (procedure)</t>
+  </si>
+  <si>
+    <t>Methanol</t>
+  </si>
+  <si>
+    <t>alcohol, methyl measurement (procedure)</t>
+  </si>
+  <si>
+    <t>Hydroxyethylflurazepam</t>
+  </si>
+  <si>
+    <t>hydroxyethylflurazepam measurement (procedure)</t>
+  </si>
+  <si>
+    <t>Hydroxyproline</t>
+  </si>
+  <si>
+    <t>hydroxyproline measurement (procedure)</t>
+  </si>
+  <si>
+    <t>Thallium</t>
+  </si>
+  <si>
+    <t>thallium measurement (procedure)</t>
+  </si>
+  <si>
+    <t>Specific gravity</t>
+  </si>
+  <si>
+    <t>specific gravity measurement (procedure)</t>
+  </si>
+  <si>
+    <t>Beta-2-Microglobulin</t>
+  </si>
+  <si>
+    <t>Beta-2-microglobulin measurement (procedure)</t>
+  </si>
+  <si>
+    <t>Antimony</t>
+  </si>
+  <si>
+    <t>antimony measurement (procedure)</t>
+  </si>
+  <si>
+    <t>Influenza virus A Ag</t>
+  </si>
+  <si>
+    <t>Influenza virus A antigen assay (procedure)</t>
+  </si>
+  <si>
+    <t>Hydroxytriazolam</t>
+  </si>
+  <si>
+    <t>hydroxytriazolam measurement (procedure)</t>
+  </si>
+  <si>
+    <t>Butabarbital</t>
+  </si>
+  <si>
+    <t>butabarbital measurement (procedure)</t>
+  </si>
+  <si>
+    <t>Bismuth</t>
+  </si>
+  <si>
+    <t>bismuth measurement (procedure)</t>
+  </si>
+  <si>
+    <t>Clobazam</t>
+  </si>
+  <si>
+    <t>clobazam measurement (procedure)</t>
+  </si>
+  <si>
+    <t>Cocaethylene</t>
+  </si>
+  <si>
+    <t>cocaethylene measurement (procedure)</t>
+  </si>
+  <si>
+    <t>Silver</t>
+  </si>
+  <si>
+    <t>silver measurement (procedure)</t>
+  </si>
+  <si>
+    <t>Molybdenum</t>
+  </si>
+  <si>
+    <t>molybdenum measurement (procedure)</t>
+  </si>
+  <si>
+    <t>Cytomegalovirus Ab</t>
+  </si>
+  <si>
+    <t>serologic test for cytomegalovirus (procedure)</t>
+  </si>
+  <si>
+    <t>Influenza virus B Ag</t>
+  </si>
+  <si>
+    <t>Influenza virus B antigen assay (procedure)</t>
+  </si>
+  <si>
+    <t>Lithium</t>
+  </si>
+  <si>
+    <t>lithium measurement (procedure)</t>
+  </si>
+  <si>
+    <t>Hydromorphone</t>
+  </si>
+  <si>
+    <t>hydromorphone measurement (procedure)</t>
+  </si>
+  <si>
+    <t>Herpes simplex virus 2 Ab.IgM</t>
+  </si>
+  <si>
+    <t>measurement of Human herpesvirus 2 antibody (procedure)</t>
+  </si>
+  <si>
+    <t>Alpha-1-Fetoprotein</t>
+  </si>
+  <si>
+    <t>alpha-1-Fetoprotein measurement (procedure)</t>
+  </si>
+  <si>
+    <t>Chlamydia trachomatis DNA</t>
+  </si>
+  <si>
+    <t>Chlamydia trachomatis deoxyribonucleic acid assay (procedure)</t>
+  </si>
+  <si>
+    <t>Fentanyl</t>
+  </si>
+  <si>
+    <t>fentanyl measurement (procedure)</t>
+  </si>
+  <si>
+    <t>Salicylates</t>
+  </si>
+  <si>
+    <t>salicylate measurement (procedure)</t>
+  </si>
+  <si>
+    <t>West Nile virus Ab.IgM</t>
+  </si>
+  <si>
+    <t>West Nile virus immunoglobulin M antibody measurement (procedure)</t>
+  </si>
+  <si>
+    <t>Methylenedioxymethamphetamine</t>
+  </si>
+  <si>
+    <t>methylenedioxymethamphetamine measurement (procedure)</t>
+  </si>
+  <si>
+    <t>Rabies virus Ab</t>
+  </si>
+  <si>
+    <t>measurement of Rabies virus antibody (procedure)</t>
+  </si>
+  <si>
+    <t>Strychnine</t>
+  </si>
+  <si>
+    <t>strychnine measurement (procedure)</t>
+  </si>
+  <si>
+    <t>Isopropanol</t>
+  </si>
+  <si>
+    <t>isopropanol measurement (procedure)</t>
+  </si>
+  <si>
+    <t>Aspergillus sp Ab</t>
+  </si>
+  <si>
+    <t>serologic test for Aspergillus (procedure)</t>
+  </si>
+  <si>
+    <t>Hydrocodone</t>
+  </si>
+  <si>
+    <t>Hydrocodone measurement (procedure)</t>
+  </si>
+  <si>
+    <t>La Crosse virus Ab.IgM</t>
+  </si>
+  <si>
+    <t>Herpes simplex virus 2 Ab</t>
+  </si>
+  <si>
+    <t>Histoplasma capsulatum Ab</t>
+  </si>
+  <si>
+    <t>measurement of Histoplasma capsulatum antibody (procedure)</t>
+  </si>
+  <si>
+    <t>Adenovirus Ab</t>
+  </si>
+  <si>
+    <t>measurement of adenovirus antibody (procedure)</t>
+  </si>
+  <si>
+    <t>Measles virus Ab.IgG</t>
+  </si>
+  <si>
+    <t>measurement of Measles virus antibody (procedure)</t>
+  </si>
+  <si>
+    <t>Estradiol</t>
+  </si>
+  <si>
+    <t>estradiol measurement (procedure)</t>
+  </si>
+  <si>
+    <t>Cortisol</t>
+  </si>
+  <si>
+    <t>cortisol measurement (procedure)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="D\-MMM\-YY;@"/>
+    <numFmt numFmtId="166" formatCode="D\-MMM\-YY;@"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -1136,6 +1389,13 @@
       <family val="0"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <b val="true"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1143,15 +1403,8 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1180,6 +1433,18 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF7030A0"/>
         <bgColor rgb="FF993366"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF767171"/>
+        <bgColor rgb="FF7C7C7C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7C7C7C"/>
+        <bgColor rgb="FF767171"/>
       </patternFill>
     </fill>
   </fills>
@@ -1283,7 +1548,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="22">
+  <cellStyleXfs count="23">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1307,7 +1572,11 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1316,12 +1585,12 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="73">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1329,7 +1598,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1345,19 +1614,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1533,7 +1802,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1541,32 +1810,85 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="22" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="5" borderId="1" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="1" xfId="22" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="21" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="22" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="3" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="3" xfId="22" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="8">
+  <cellStyles count="9">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Normal_LOINC Rules" xfId="20" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Normal 2" xfId="21" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Normal_LOINC Rules" xfId="20" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Normal_LOINC Rules" xfId="21" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Normal 2" xfId="22" builtinId="54" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -1585,7 +1907,7 @@
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFC5E0B4"/>
-      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF7C7C7C"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF7030A0"/>
       <rgbColor rgb="FFFFFFCC"/>
@@ -1616,7 +1938,7 @@
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
-      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF767171"/>
       <rgbColor rgb="FF969696"/>
       <rgbColor rgb="FF003366"/>
       <rgbColor rgb="FF339966"/>
@@ -1753,16 +2075,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:BB166"/>
+  <dimension ref="A1:BB223"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A145" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B169" activeCellId="0" sqref="B169"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A184" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A224" activeCellId="0" sqref="A224"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.53441295546559"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.4251012145749"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.53441295546559"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="4" width="9.1417004048583"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.8542510121457"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="52.4251012145749"/>
@@ -9148,6 +9471,1578 @@
         <v>28</v>
       </c>
     </row>
+    <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A167" s="45"/>
+      <c r="B167" s="60"/>
+      <c r="C167" s="60"/>
+      <c r="D167" s="47"/>
+      <c r="E167" s="45"/>
+      <c r="F167" s="61"/>
+      <c r="G167" s="45"/>
+      <c r="H167" s="45"/>
+      <c r="I167" s="45"/>
+      <c r="J167" s="45"/>
+      <c r="K167" s="45"/>
+      <c r="L167" s="45"/>
+    </row>
+    <row r="168" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A168" s="50" t="n">
+        <v>2115</v>
+      </c>
+      <c r="B168" s="62" t="n">
+        <v>42139</v>
+      </c>
+      <c r="C168" s="62"/>
+      <c r="D168" s="52"/>
+      <c r="E168" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F168" s="63" t="s">
+        <v>362</v>
+      </c>
+      <c r="G168" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H168" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I168" s="50" t="n">
+        <v>113055007</v>
+      </c>
+      <c r="J168" s="50" t="s">
+        <v>363</v>
+      </c>
+      <c r="K168" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L168" s="50"/>
+    </row>
+    <row r="169" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A169" s="50" t="n">
+        <v>2116</v>
+      </c>
+      <c r="B169" s="62" t="n">
+        <v>42139</v>
+      </c>
+      <c r="C169" s="62"/>
+      <c r="D169" s="52"/>
+      <c r="E169" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F169" s="63" t="s">
+        <v>364</v>
+      </c>
+      <c r="G169" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H169" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I169" s="50" t="n">
+        <v>122330002</v>
+      </c>
+      <c r="J169" s="50" t="s">
+        <v>365</v>
+      </c>
+      <c r="K169" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L169" s="50"/>
+    </row>
+    <row r="170" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A170" s="64"/>
+      <c r="B170" s="65"/>
+      <c r="C170" s="65"/>
+      <c r="D170" s="66"/>
+      <c r="E170" s="64"/>
+      <c r="F170" s="67"/>
+      <c r="G170" s="64"/>
+      <c r="H170" s="64"/>
+      <c r="I170" s="64"/>
+      <c r="J170" s="64"/>
+      <c r="K170" s="64"/>
+      <c r="L170" s="64"/>
+    </row>
+    <row r="171" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A171" s="50" t="n">
+        <v>2118</v>
+      </c>
+      <c r="B171" s="62" t="n">
+        <v>42139</v>
+      </c>
+      <c r="C171" s="62"/>
+      <c r="D171" s="52"/>
+      <c r="E171" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F171" s="63" t="s">
+        <v>366</v>
+      </c>
+      <c r="G171" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H171" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I171" s="50" t="n">
+        <v>26052003</v>
+      </c>
+      <c r="J171" s="50" t="s">
+        <v>367</v>
+      </c>
+      <c r="K171" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L171" s="50"/>
+    </row>
+    <row r="172" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A172" s="50" t="n">
+        <v>2119</v>
+      </c>
+      <c r="B172" s="62" t="n">
+        <v>42139</v>
+      </c>
+      <c r="C172" s="62"/>
+      <c r="D172" s="52"/>
+      <c r="E172" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F172" s="63" t="s">
+        <v>368</v>
+      </c>
+      <c r="G172" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H172" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I172" s="50" t="n">
+        <v>36174000</v>
+      </c>
+      <c r="J172" s="50" t="s">
+        <v>369</v>
+      </c>
+      <c r="K172" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L172" s="50"/>
+    </row>
+    <row r="173" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A173" s="50" t="n">
+        <v>2120</v>
+      </c>
+      <c r="B173" s="62" t="n">
+        <v>42139</v>
+      </c>
+      <c r="C173" s="62"/>
+      <c r="D173" s="52"/>
+      <c r="E173" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F173" s="63" t="s">
+        <v>370</v>
+      </c>
+      <c r="G173" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H173" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I173" s="50" t="n">
+        <v>122017008</v>
+      </c>
+      <c r="J173" s="50" t="s">
+        <v>371</v>
+      </c>
+      <c r="K173" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L173" s="50"/>
+    </row>
+    <row r="174" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A174" s="50" t="n">
+        <v>2121</v>
+      </c>
+      <c r="B174" s="62" t="n">
+        <v>42139</v>
+      </c>
+      <c r="C174" s="62"/>
+      <c r="D174" s="52"/>
+      <c r="E174" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F174" s="63" t="s">
+        <v>372</v>
+      </c>
+      <c r="G174" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H174" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I174" s="50" t="n">
+        <v>57582005</v>
+      </c>
+      <c r="J174" s="50" t="s">
+        <v>373</v>
+      </c>
+      <c r="K174" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L174" s="50"/>
+    </row>
+    <row r="175" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A175" s="50" t="n">
+        <v>2122</v>
+      </c>
+      <c r="B175" s="62" t="n">
+        <v>42139</v>
+      </c>
+      <c r="C175" s="62"/>
+      <c r="D175" s="52"/>
+      <c r="E175" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F175" s="63" t="s">
+        <v>374</v>
+      </c>
+      <c r="G175" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H175" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I175" s="50" t="n">
+        <v>121602006</v>
+      </c>
+      <c r="J175" s="50" t="s">
+        <v>375</v>
+      </c>
+      <c r="K175" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L175" s="50"/>
+    </row>
+    <row r="176" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A176" s="50" t="n">
+        <v>2123</v>
+      </c>
+      <c r="B176" s="62" t="n">
+        <v>42139</v>
+      </c>
+      <c r="C176" s="62"/>
+      <c r="D176" s="52"/>
+      <c r="E176" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F176" s="63" t="s">
+        <v>376</v>
+      </c>
+      <c r="G176" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H176" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I176" s="50" t="n">
+        <v>55112008</v>
+      </c>
+      <c r="J176" s="50" t="s">
+        <v>377</v>
+      </c>
+      <c r="K176" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L176" s="50"/>
+    </row>
+    <row r="177" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A177" s="64"/>
+      <c r="B177" s="65"/>
+      <c r="C177" s="65"/>
+      <c r="D177" s="66"/>
+      <c r="E177" s="64"/>
+      <c r="F177" s="67"/>
+      <c r="G177" s="64"/>
+      <c r="H177" s="64"/>
+      <c r="I177" s="64"/>
+      <c r="J177" s="64"/>
+      <c r="K177" s="64"/>
+      <c r="L177" s="64"/>
+    </row>
+    <row r="178" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A178" s="50" t="n">
+        <v>2125</v>
+      </c>
+      <c r="B178" s="62" t="n">
+        <v>42139</v>
+      </c>
+      <c r="C178" s="62"/>
+      <c r="D178" s="52"/>
+      <c r="E178" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F178" s="63" t="s">
+        <v>378</v>
+      </c>
+      <c r="G178" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H178" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I178" s="50" t="n">
+        <v>105336005</v>
+      </c>
+      <c r="J178" s="50" t="s">
+        <v>379</v>
+      </c>
+      <c r="K178" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L178" s="50"/>
+    </row>
+    <row r="179" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A179" s="64"/>
+      <c r="B179" s="65"/>
+      <c r="C179" s="65"/>
+      <c r="D179" s="66"/>
+      <c r="E179" s="64"/>
+      <c r="F179" s="67"/>
+      <c r="G179" s="64"/>
+      <c r="H179" s="64"/>
+      <c r="I179" s="64"/>
+      <c r="J179" s="64"/>
+      <c r="K179" s="64"/>
+      <c r="L179" s="64"/>
+    </row>
+    <row r="180" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A180" s="50" t="n">
+        <v>2127</v>
+      </c>
+      <c r="B180" s="62" t="n">
+        <v>42139</v>
+      </c>
+      <c r="C180" s="62"/>
+      <c r="D180" s="52"/>
+      <c r="E180" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F180" s="63" t="s">
+        <v>380</v>
+      </c>
+      <c r="G180" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H180" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I180" s="50" t="n">
+        <v>69285004</v>
+      </c>
+      <c r="J180" s="50" t="s">
+        <v>381</v>
+      </c>
+      <c r="K180" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L180" s="50"/>
+    </row>
+    <row r="181" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A181" s="64"/>
+      <c r="B181" s="65"/>
+      <c r="C181" s="65"/>
+      <c r="D181" s="66"/>
+      <c r="E181" s="64"/>
+      <c r="F181" s="67"/>
+      <c r="G181" s="64"/>
+      <c r="H181" s="64"/>
+      <c r="I181" s="64"/>
+      <c r="J181" s="64"/>
+      <c r="K181" s="64"/>
+      <c r="L181" s="64"/>
+    </row>
+    <row r="182" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A182" s="50" t="n">
+        <v>2129</v>
+      </c>
+      <c r="B182" s="62" t="n">
+        <v>42139</v>
+      </c>
+      <c r="C182" s="62"/>
+      <c r="D182" s="52"/>
+      <c r="E182" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F182" s="63" t="s">
+        <v>382</v>
+      </c>
+      <c r="G182" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H182" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I182" s="50" t="n">
+        <v>81410005</v>
+      </c>
+      <c r="J182" s="50" t="s">
+        <v>383</v>
+      </c>
+      <c r="K182" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L182" s="50"/>
+    </row>
+    <row r="183" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A183" s="50" t="n">
+        <v>2130</v>
+      </c>
+      <c r="B183" s="62" t="n">
+        <v>42139</v>
+      </c>
+      <c r="C183" s="62"/>
+      <c r="D183" s="52"/>
+      <c r="E183" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F183" s="63" t="s">
+        <v>384</v>
+      </c>
+      <c r="G183" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H183" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I183" s="50" t="n">
+        <v>43388004</v>
+      </c>
+      <c r="J183" s="50" t="s">
+        <v>385</v>
+      </c>
+      <c r="K183" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L183" s="50"/>
+    </row>
+    <row r="184" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A184" s="64"/>
+      <c r="B184" s="65"/>
+      <c r="C184" s="65"/>
+      <c r="D184" s="66"/>
+      <c r="E184" s="64"/>
+      <c r="F184" s="67"/>
+      <c r="G184" s="64"/>
+      <c r="H184" s="64"/>
+      <c r="I184" s="64"/>
+      <c r="J184" s="64"/>
+      <c r="K184" s="64"/>
+      <c r="L184" s="64"/>
+    </row>
+    <row r="185" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A185" s="50" t="n">
+        <v>2132</v>
+      </c>
+      <c r="B185" s="62" t="n">
+        <v>42139</v>
+      </c>
+      <c r="C185" s="62"/>
+      <c r="D185" s="52"/>
+      <c r="E185" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F185" s="63" t="s">
+        <v>386</v>
+      </c>
+      <c r="G185" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H185" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I185" s="50" t="n">
+        <v>122349003</v>
+      </c>
+      <c r="J185" s="50" t="s">
+        <v>387</v>
+      </c>
+      <c r="K185" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L185" s="50"/>
+    </row>
+    <row r="186" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A186" s="50" t="n">
+        <v>2133</v>
+      </c>
+      <c r="B186" s="62" t="n">
+        <v>42139</v>
+      </c>
+      <c r="C186" s="62"/>
+      <c r="D186" s="52"/>
+      <c r="E186" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F186" s="63" t="s">
+        <v>388</v>
+      </c>
+      <c r="G186" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H186" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I186" s="50" t="n">
+        <v>121603001</v>
+      </c>
+      <c r="J186" s="50" t="s">
+        <v>389</v>
+      </c>
+      <c r="K186" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L186" s="50"/>
+    </row>
+    <row r="187" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A187" s="50" t="n">
+        <v>2134</v>
+      </c>
+      <c r="B187" s="62" t="n">
+        <v>42139</v>
+      </c>
+      <c r="C187" s="62"/>
+      <c r="D187" s="52"/>
+      <c r="E187" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F187" s="63" t="s">
+        <v>390</v>
+      </c>
+      <c r="G187" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H187" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I187" s="50" t="n">
+        <v>56919009</v>
+      </c>
+      <c r="J187" s="50" t="s">
+        <v>391</v>
+      </c>
+      <c r="K187" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L187" s="50"/>
+    </row>
+    <row r="188" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A188" s="50" t="n">
+        <v>2135</v>
+      </c>
+      <c r="B188" s="62" t="n">
+        <v>42139</v>
+      </c>
+      <c r="C188" s="62"/>
+      <c r="D188" s="52"/>
+      <c r="E188" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F188" s="63" t="s">
+        <v>392</v>
+      </c>
+      <c r="G188" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H188" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I188" s="50" t="n">
+        <v>64685008</v>
+      </c>
+      <c r="J188" s="50" t="s">
+        <v>393</v>
+      </c>
+      <c r="K188" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L188" s="50"/>
+    </row>
+    <row r="189" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A189" s="50" t="n">
+        <v>2136</v>
+      </c>
+      <c r="B189" s="62" t="n">
+        <v>42139</v>
+      </c>
+      <c r="C189" s="62"/>
+      <c r="D189" s="52"/>
+      <c r="E189" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F189" s="63" t="s">
+        <v>394</v>
+      </c>
+      <c r="G189" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H189" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I189" s="50" t="n">
+        <v>105131008</v>
+      </c>
+      <c r="J189" s="50" t="s">
+        <v>395</v>
+      </c>
+      <c r="K189" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L189" s="50"/>
+    </row>
+    <row r="190" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A190" s="50" t="n">
+        <v>2137</v>
+      </c>
+      <c r="B190" s="62" t="n">
+        <v>42139</v>
+      </c>
+      <c r="C190" s="62"/>
+      <c r="D190" s="52"/>
+      <c r="E190" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F190" s="63" t="s">
+        <v>396</v>
+      </c>
+      <c r="G190" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H190" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I190" s="50" t="n">
+        <v>121505002</v>
+      </c>
+      <c r="J190" s="50" t="s">
+        <v>397</v>
+      </c>
+      <c r="K190" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L190" s="50"/>
+    </row>
+    <row r="191" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A191" s="50" t="n">
+        <v>2138</v>
+      </c>
+      <c r="B191" s="62" t="n">
+        <v>42139</v>
+      </c>
+      <c r="C191" s="62"/>
+      <c r="D191" s="52"/>
+      <c r="E191" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F191" s="63" t="s">
+        <v>398</v>
+      </c>
+      <c r="G191" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H191" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I191" s="50" t="n">
+        <v>32464007</v>
+      </c>
+      <c r="J191" s="50" t="s">
+        <v>399</v>
+      </c>
+      <c r="K191" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L191" s="50"/>
+    </row>
+    <row r="192" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A192" s="64"/>
+      <c r="B192" s="65"/>
+      <c r="C192" s="65"/>
+      <c r="D192" s="66"/>
+      <c r="E192" s="64"/>
+      <c r="F192" s="67"/>
+      <c r="G192" s="64"/>
+      <c r="H192" s="64"/>
+      <c r="I192" s="64"/>
+      <c r="J192" s="64"/>
+      <c r="K192" s="64"/>
+      <c r="L192" s="64"/>
+    </row>
+    <row r="193" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A193" s="64"/>
+      <c r="B193" s="65"/>
+      <c r="C193" s="65"/>
+      <c r="D193" s="66"/>
+      <c r="E193" s="64"/>
+      <c r="F193" s="67"/>
+      <c r="G193" s="64"/>
+      <c r="H193" s="64"/>
+      <c r="I193" s="64"/>
+      <c r="J193" s="64"/>
+      <c r="K193" s="64"/>
+      <c r="L193" s="64"/>
+    </row>
+    <row r="194" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A194" s="50" t="n">
+        <v>2141</v>
+      </c>
+      <c r="B194" s="62" t="n">
+        <v>42139</v>
+      </c>
+      <c r="C194" s="62"/>
+      <c r="D194" s="52"/>
+      <c r="E194" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F194" s="63" t="s">
+        <v>400</v>
+      </c>
+      <c r="G194" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H194" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I194" s="50" t="n">
+        <v>61065009</v>
+      </c>
+      <c r="J194" s="50" t="s">
+        <v>401</v>
+      </c>
+      <c r="K194" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L194" s="50"/>
+    </row>
+    <row r="195" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A195" s="50" t="n">
+        <v>2142</v>
+      </c>
+      <c r="B195" s="62" t="n">
+        <v>42139</v>
+      </c>
+      <c r="C195" s="62"/>
+      <c r="D195" s="52"/>
+      <c r="E195" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F195" s="63" t="s">
+        <v>402</v>
+      </c>
+      <c r="G195" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H195" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I195" s="50" t="n">
+        <v>30200007</v>
+      </c>
+      <c r="J195" s="50" t="s">
+        <v>403</v>
+      </c>
+      <c r="K195" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L195" s="50"/>
+    </row>
+    <row r="196" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A196" s="50" t="n">
+        <v>2143</v>
+      </c>
+      <c r="B196" s="62" t="n">
+        <v>42139</v>
+      </c>
+      <c r="C196" s="62"/>
+      <c r="D196" s="52"/>
+      <c r="E196" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F196" s="63" t="s">
+        <v>404</v>
+      </c>
+      <c r="G196" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H196" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I196" s="50" t="n">
+        <v>122350003</v>
+      </c>
+      <c r="J196" s="50" t="s">
+        <v>405</v>
+      </c>
+      <c r="K196" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L196" s="50"/>
+    </row>
+    <row r="197" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A197" s="64"/>
+      <c r="B197" s="65"/>
+      <c r="C197" s="65"/>
+      <c r="D197" s="66"/>
+      <c r="E197" s="64"/>
+      <c r="F197" s="67"/>
+      <c r="G197" s="64"/>
+      <c r="H197" s="64"/>
+      <c r="I197" s="64"/>
+      <c r="J197" s="64"/>
+      <c r="K197" s="64"/>
+      <c r="L197" s="64"/>
+    </row>
+    <row r="198" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A198" s="50" t="n">
+        <v>2145</v>
+      </c>
+      <c r="B198" s="62" t="n">
+        <v>42139</v>
+      </c>
+      <c r="C198" s="62"/>
+      <c r="D198" s="52"/>
+      <c r="E198" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F198" s="63" t="s">
+        <v>406</v>
+      </c>
+      <c r="G198" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H198" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I198" s="50" t="n">
+        <v>54392006</v>
+      </c>
+      <c r="J198" s="50" t="s">
+        <v>407</v>
+      </c>
+      <c r="K198" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L198" s="50"/>
+    </row>
+    <row r="199" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A199" s="50" t="n">
+        <v>2146</v>
+      </c>
+      <c r="B199" s="62" t="n">
+        <v>42139</v>
+      </c>
+      <c r="C199" s="62"/>
+      <c r="D199" s="52"/>
+      <c r="E199" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F199" s="63" t="s">
+        <v>408</v>
+      </c>
+      <c r="G199" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H199" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I199" s="50" t="n">
+        <v>105207008</v>
+      </c>
+      <c r="J199" s="50" t="s">
+        <v>409</v>
+      </c>
+      <c r="K199" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L199" s="50"/>
+    </row>
+    <row r="200" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A200" s="68" t="n">
+        <v>2147</v>
+      </c>
+      <c r="B200" s="62" t="n">
+        <v>42139</v>
+      </c>
+      <c r="C200" s="62"/>
+      <c r="D200" s="52"/>
+      <c r="E200" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F200" s="63" t="s">
+        <v>410</v>
+      </c>
+      <c r="G200" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H200" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I200" s="50" t="n">
+        <v>117739006</v>
+      </c>
+      <c r="J200" s="50" t="s">
+        <v>411</v>
+      </c>
+      <c r="K200" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L200" s="50"/>
+    </row>
+    <row r="201" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A201" s="50" t="n">
+        <v>2148</v>
+      </c>
+      <c r="B201" s="62" t="n">
+        <v>42139</v>
+      </c>
+      <c r="C201" s="62"/>
+      <c r="D201" s="52"/>
+      <c r="E201" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F201" s="63" t="s">
+        <v>412</v>
+      </c>
+      <c r="G201" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H201" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I201" s="50" t="n">
+        <v>80152001</v>
+      </c>
+      <c r="J201" s="50" t="s">
+        <v>413</v>
+      </c>
+      <c r="K201" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L201" s="50"/>
+    </row>
+    <row r="202" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A202" s="50" t="n">
+        <v>2149</v>
+      </c>
+      <c r="B202" s="62" t="n">
+        <v>42139</v>
+      </c>
+      <c r="C202" s="62"/>
+      <c r="D202" s="52"/>
+      <c r="E202" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F202" s="63" t="s">
+        <v>414</v>
+      </c>
+      <c r="G202" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H202" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I202" s="50" t="n">
+        <v>122321005</v>
+      </c>
+      <c r="J202" s="50" t="s">
+        <v>415</v>
+      </c>
+      <c r="K202" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L202" s="50"/>
+    </row>
+    <row r="203" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A203" s="50" t="n">
+        <v>2150</v>
+      </c>
+      <c r="B203" s="62" t="n">
+        <v>42139</v>
+      </c>
+      <c r="C203" s="62"/>
+      <c r="D203" s="52"/>
+      <c r="E203" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F203" s="63" t="s">
+        <v>416</v>
+      </c>
+      <c r="G203" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H203" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I203" s="50" t="n">
+        <v>105192003</v>
+      </c>
+      <c r="J203" s="50" t="s">
+        <v>417</v>
+      </c>
+      <c r="K203" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L203" s="50"/>
+    </row>
+    <row r="204" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A204" s="50" t="n">
+        <v>2151</v>
+      </c>
+      <c r="B204" s="62" t="n">
+        <v>42139</v>
+      </c>
+      <c r="C204" s="62"/>
+      <c r="D204" s="52"/>
+      <c r="E204" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F204" s="63" t="s">
+        <v>418</v>
+      </c>
+      <c r="G204" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H204" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I204" s="50" t="n">
+        <v>36206007</v>
+      </c>
+      <c r="J204" s="50" t="s">
+        <v>419</v>
+      </c>
+      <c r="K204" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L204" s="50"/>
+    </row>
+    <row r="205" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A205" s="50" t="n">
+        <v>2152</v>
+      </c>
+      <c r="B205" s="62" t="n">
+        <v>42139</v>
+      </c>
+      <c r="C205" s="62"/>
+      <c r="D205" s="52"/>
+      <c r="E205" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F205" s="63" t="s">
+        <v>420</v>
+      </c>
+      <c r="G205" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H205" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I205" s="50" t="n">
+        <v>420880005</v>
+      </c>
+      <c r="J205" s="50" t="s">
+        <v>421</v>
+      </c>
+      <c r="K205" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L205" s="50"/>
+    </row>
+    <row r="206" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A206" s="69"/>
+      <c r="B206" s="70"/>
+      <c r="C206" s="70"/>
+      <c r="D206" s="71"/>
+      <c r="E206" s="69"/>
+      <c r="F206" s="72"/>
+      <c r="G206" s="69"/>
+      <c r="H206" s="69"/>
+      <c r="I206" s="69"/>
+      <c r="J206" s="69"/>
+      <c r="K206" s="69"/>
+      <c r="L206" s="69"/>
+    </row>
+    <row r="207" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A207" s="69"/>
+      <c r="B207" s="70"/>
+      <c r="C207" s="70"/>
+      <c r="D207" s="71"/>
+      <c r="E207" s="69"/>
+      <c r="F207" s="72"/>
+      <c r="G207" s="69"/>
+      <c r="H207" s="69"/>
+      <c r="I207" s="69"/>
+      <c r="J207" s="69"/>
+      <c r="K207" s="69"/>
+      <c r="L207" s="69"/>
+    </row>
+    <row r="208" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A208" s="50" t="n">
+        <v>2155</v>
+      </c>
+      <c r="B208" s="62" t="n">
+        <v>42139</v>
+      </c>
+      <c r="C208" s="62"/>
+      <c r="D208" s="52"/>
+      <c r="E208" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F208" s="63" t="s">
+        <v>422</v>
+      </c>
+      <c r="G208" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H208" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I208" s="50" t="n">
+        <v>121373009</v>
+      </c>
+      <c r="J208" s="50" t="s">
+        <v>423</v>
+      </c>
+      <c r="K208" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L208" s="50"/>
+    </row>
+    <row r="209" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A209" s="50" t="n">
+        <v>2156</v>
+      </c>
+      <c r="B209" s="62" t="n">
+        <v>42139</v>
+      </c>
+      <c r="C209" s="62"/>
+      <c r="D209" s="52"/>
+      <c r="E209" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F209" s="63" t="s">
+        <v>424</v>
+      </c>
+      <c r="G209" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H209" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I209" s="50" t="n">
+        <v>122078009</v>
+      </c>
+      <c r="J209" s="50" t="s">
+        <v>425</v>
+      </c>
+      <c r="K209" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L209" s="50"/>
+    </row>
+    <row r="210" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A210" s="50" t="n">
+        <v>2157</v>
+      </c>
+      <c r="B210" s="62" t="n">
+        <v>42139</v>
+      </c>
+      <c r="C210" s="62"/>
+      <c r="D210" s="52"/>
+      <c r="E210" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F210" s="63" t="s">
+        <v>426</v>
+      </c>
+      <c r="G210" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H210" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I210" s="50" t="n">
+        <v>71167000</v>
+      </c>
+      <c r="J210" s="50" t="s">
+        <v>427</v>
+      </c>
+      <c r="K210" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L210" s="50"/>
+    </row>
+    <row r="211" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A211" s="69"/>
+      <c r="B211" s="70"/>
+      <c r="C211" s="70"/>
+      <c r="D211" s="71"/>
+      <c r="E211" s="69"/>
+      <c r="F211" s="72"/>
+      <c r="G211" s="69"/>
+      <c r="H211" s="69"/>
+      <c r="I211" s="69"/>
+      <c r="J211" s="69"/>
+      <c r="K211" s="69"/>
+      <c r="L211" s="69"/>
+    </row>
+    <row r="212" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A212" s="50" t="n">
+        <v>2159</v>
+      </c>
+      <c r="B212" s="62" t="n">
+        <v>42139</v>
+      </c>
+      <c r="C212" s="62"/>
+      <c r="D212" s="52"/>
+      <c r="E212" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F212" s="63" t="s">
+        <v>428</v>
+      </c>
+      <c r="G212" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H212" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I212" s="50" t="n">
+        <v>105217003</v>
+      </c>
+      <c r="J212" s="50" t="s">
+        <v>429</v>
+      </c>
+      <c r="K212" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L212" s="50"/>
+    </row>
+    <row r="213" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A213" s="50" t="n">
+        <v>2160</v>
+      </c>
+      <c r="B213" s="62" t="n">
+        <v>42139</v>
+      </c>
+      <c r="C213" s="62"/>
+      <c r="D213" s="52"/>
+      <c r="E213" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F213" s="63" t="s">
+        <v>430</v>
+      </c>
+      <c r="G213" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H213" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I213" s="50" t="n">
+        <v>87407009</v>
+      </c>
+      <c r="J213" s="50" t="s">
+        <v>431</v>
+      </c>
+      <c r="K213" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L213" s="50"/>
+    </row>
+    <row r="214" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A214" s="50" t="n">
+        <v>2161</v>
+      </c>
+      <c r="B214" s="62" t="n">
+        <v>42139</v>
+      </c>
+      <c r="C214" s="62"/>
+      <c r="D214" s="52"/>
+      <c r="E214" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F214" s="63" t="s">
+        <v>432</v>
+      </c>
+      <c r="G214" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H214" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I214" s="50" t="n">
+        <v>105206004</v>
+      </c>
+      <c r="J214" s="50" t="s">
+        <v>433</v>
+      </c>
+      <c r="K214" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L214" s="50"/>
+    </row>
+    <row r="215" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A215" s="68" t="n">
+        <v>2162</v>
+      </c>
+      <c r="B215" s="62" t="n">
+        <v>42139</v>
+      </c>
+      <c r="C215" s="62"/>
+      <c r="D215" s="52"/>
+      <c r="E215" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F215" s="63" t="s">
+        <v>434</v>
+      </c>
+      <c r="G215" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H215" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I215" s="50" t="n">
+        <v>122017008</v>
+      </c>
+      <c r="J215" s="50" t="s">
+        <v>371</v>
+      </c>
+      <c r="K215" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L215" s="50"/>
+    </row>
+    <row r="216" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A216" s="50" t="n">
+        <v>2163</v>
+      </c>
+      <c r="B216" s="62" t="n">
+        <v>42139</v>
+      </c>
+      <c r="C216" s="62"/>
+      <c r="D216" s="52"/>
+      <c r="E216" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F216" s="63" t="s">
+        <v>435</v>
+      </c>
+      <c r="G216" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H216" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I216" s="50" t="n">
+        <v>117739006</v>
+      </c>
+      <c r="J216" s="50" t="s">
+        <v>411</v>
+      </c>
+      <c r="K216" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L216" s="50"/>
+    </row>
+    <row r="217" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A217" s="50" t="n">
+        <v>2164</v>
+      </c>
+      <c r="B217" s="62" t="n">
+        <v>42139</v>
+      </c>
+      <c r="C217" s="62"/>
+      <c r="D217" s="52"/>
+      <c r="E217" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F217" s="63" t="s">
+        <v>436</v>
+      </c>
+      <c r="G217" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H217" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I217" s="50" t="n">
+        <v>121914001</v>
+      </c>
+      <c r="J217" s="50" t="s">
+        <v>437</v>
+      </c>
+      <c r="K217" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L217" s="50"/>
+    </row>
+    <row r="218" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A218" s="64"/>
+      <c r="B218" s="65"/>
+      <c r="C218" s="65"/>
+      <c r="D218" s="66"/>
+      <c r="E218" s="64"/>
+      <c r="F218" s="67"/>
+      <c r="G218" s="64"/>
+      <c r="H218" s="64"/>
+      <c r="I218" s="64"/>
+      <c r="J218" s="64"/>
+      <c r="K218" s="64"/>
+      <c r="L218" s="64"/>
+    </row>
+    <row r="219" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A219" s="64"/>
+      <c r="B219" s="65"/>
+      <c r="C219" s="65"/>
+      <c r="D219" s="66"/>
+      <c r="E219" s="64"/>
+      <c r="F219" s="67"/>
+      <c r="G219" s="64"/>
+      <c r="H219" s="64"/>
+      <c r="I219" s="64"/>
+      <c r="J219" s="64"/>
+      <c r="K219" s="64"/>
+      <c r="L219" s="64"/>
+    </row>
+    <row r="220" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A220" s="50" t="n">
+        <v>2167</v>
+      </c>
+      <c r="B220" s="62" t="n">
+        <v>42139</v>
+      </c>
+      <c r="C220" s="62"/>
+      <c r="D220" s="52"/>
+      <c r="E220" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F220" s="63" t="s">
+        <v>438</v>
+      </c>
+      <c r="G220" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H220" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I220" s="50" t="n">
+        <v>104311005</v>
+      </c>
+      <c r="J220" s="50" t="s">
+        <v>439</v>
+      </c>
+      <c r="K220" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L220" s="50"/>
+    </row>
+    <row r="221" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A221" s="50" t="n">
+        <v>2168</v>
+      </c>
+      <c r="B221" s="62" t="n">
+        <v>42139</v>
+      </c>
+      <c r="C221" s="62"/>
+      <c r="D221" s="52"/>
+      <c r="E221" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F221" s="63" t="s">
+        <v>440</v>
+      </c>
+      <c r="G221" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H221" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I221" s="50" t="n">
+        <v>104325006</v>
+      </c>
+      <c r="J221" s="50" t="s">
+        <v>441</v>
+      </c>
+      <c r="K221" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L221" s="50"/>
+    </row>
+    <row r="222" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A222" s="50" t="n">
+        <v>2169</v>
+      </c>
+      <c r="B222" s="62" t="n">
+        <v>42139</v>
+      </c>
+      <c r="C222" s="62"/>
+      <c r="D222" s="52"/>
+      <c r="E222" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F222" s="63" t="s">
+        <v>442</v>
+      </c>
+      <c r="G222" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H222" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I222" s="50" t="n">
+        <v>37538009</v>
+      </c>
+      <c r="J222" s="50" t="s">
+        <v>443</v>
+      </c>
+      <c r="K222" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L222" s="50"/>
+    </row>
+    <row r="223" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A223" s="50" t="n">
+        <v>2170</v>
+      </c>
+      <c r="B223" s="62" t="n">
+        <v>42140</v>
+      </c>
+      <c r="C223" s="62"/>
+      <c r="D223" s="52"/>
+      <c r="E223" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F223" s="63" t="s">
+        <v>444</v>
+      </c>
+      <c r="G223" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H223" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I223" s="50" t="n">
+        <v>62037009</v>
+      </c>
+      <c r="J223" s="50" t="s">
+        <v>445</v>
+      </c>
+      <c r="K223" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="L223" s="50"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:G1"/>

</xml_diff>